<commit_message>
1. add ep factory
</commit_message>
<xml_diff>
--- a/src/test/resources/com/github/zhangchunsheng/excel2pdf/sample1/case1.xlsx
+++ b/src/test/resources/com/github/zhangchunsheng/excel2pdf/sample1/case1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterzhang/dev/github/excel-to-pdf/src/test/resources/com/github/zhangchunsheng/excel2pdf/sample1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B9C7AEA-55E4-D346-ACED-63532D30B3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CE93EE-DE80-5740-ADBD-9BCF06B0FF99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14660"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,20 +18,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="114210"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="43">
   <si>
     <t>加班開始</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -166,12 +157,15 @@
   <si>
     <t>姓    名：陳XX</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
       <sz val="12"/>
@@ -285,7 +279,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -325,6 +319,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -639,14 +636,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1140,6 +1137,11 @@
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="C24" s="14" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1157,7 +1159,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1174,7 +1176,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>